<commit_message>
chantier html et depot des trucs faits dans le pptx
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO (1).xlsx
+++ b/Modèle-audit-SEO (1).xlsx
@@ -48,12 +48,6 @@
     <t>structure html</t>
   </si>
   <si>
-    <t>Structure div only</t>
-  </si>
-  <si>
-    <t>utilisation des balises sémantiques (main header footer, etc)</t>
-  </si>
-  <si>
     <t>SEO</t>
   </si>
   <si>
@@ -190,6 +184,12 @@
   </si>
   <si>
     <t>Eviter les images pour du texte</t>
+  </si>
+  <si>
+    <t>Structure div only + lang=default</t>
+  </si>
+  <si>
+    <t>utilisation des balises sémantiques (main header footer, etc) lang=fr</t>
   </si>
 </sst>
 </file>
@@ -521,7 +521,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1"/>
@@ -577,44 +577,44 @@
     </row>
     <row r="2" spans="1:26" s="12" customFormat="1" ht="30">
       <c r="A2" s="13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="E2" s="8" t="s">
         <v>51</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="D3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:26">
       <c r="A4" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -622,167 +622,167 @@
     </row>
     <row r="5" spans="1:26" ht="30">
       <c r="A5" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="E5" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="30">
       <c r="A6" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="30">
       <c r="A7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="E7" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="30">
       <c r="A8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="D8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="30">
       <c r="A9" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="30">
       <c r="A10" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="60">
       <c r="A11" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="45">
       <c r="A12" s="9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1">
       <c r="B15" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E15" s="3"/>
     </row>

</xml_diff>